<commit_message>
Read in external weight files
</commit_message>
<xml_diff>
--- a/src/consequenceTypes.xlsx
+++ b/src/consequenceTypes.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dave\OneDrive\msvc\geneVarAssocGit\geneVarAssoc\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dave_000\OneDrive\msvc\geneVarAssocGit\geneVarAssoc\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9510" windowHeight="3840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9516" windowHeight="3840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="171">
   <si>
     <t>*</t>
   </si>
@@ -520,7 +522,25 @@
     <t>KOZAK</t>
   </si>
   <si>
-    <t xml:space="preserve">On 29/12/18, from http://www.ensembl.org/info/genome/variation/predicted_data.html#consequences </t>
+    <t xml:space="preserve">On 29/12/16, from http://www.ensembl.org/info/genome/variation/predicted_data.html#consequences </t>
+  </si>
+  <si>
+    <t>ConsequenceType</t>
+  </si>
+  <si>
+    <t>ConsequenceLevel</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>ConsequenceEnum</t>
+  </si>
+  <si>
+    <t>CodeForStructure</t>
+  </si>
+  <si>
+    <t>CodeForEnum</t>
   </si>
 </sst>
 </file>
@@ -1067,24 +1087,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="40.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" customWidth="1"/>
-    <col min="6" max="6" width="44.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.88671875" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" customWidth="1"/>
+    <col min="5" max="5" width="23.109375" customWidth="1"/>
+    <col min="6" max="6" width="44.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1104,7 +1124,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="3" t="s">
         <v>6</v>
@@ -1122,7 +1142,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="3" t="s">
         <v>11</v>
@@ -1140,7 +1160,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="3" t="s">
         <v>15</v>
@@ -1158,7 +1178,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="3" t="s">
         <v>19</v>
@@ -1176,7 +1196,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" s="3" t="s">
         <v>23</v>
@@ -1194,7 +1214,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="3" t="s">
         <v>27</v>
@@ -1212,7 +1232,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="3" t="s">
         <v>31</v>
@@ -1230,7 +1250,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="B11" s="3" t="s">
         <v>35</v>
@@ -1248,7 +1268,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="3" t="s">
         <v>39</v>
@@ -1266,7 +1286,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="3" t="s">
         <v>44</v>
@@ -1284,7 +1304,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="3" t="s">
         <v>48</v>
@@ -1302,7 +1322,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
       <c r="B15" s="3" t="s">
         <v>52</v>
@@ -1320,7 +1340,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A16" s="12"/>
       <c r="B16" s="3" t="s">
         <v>56</v>
@@ -1338,7 +1358,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="13"/>
       <c r="B17" s="3" t="s">
         <v>61</v>
@@ -1356,7 +1376,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="3" t="s">
         <v>65</v>
@@ -1374,7 +1394,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="3" t="s">
         <v>69</v>
@@ -1392,7 +1412,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="15"/>
       <c r="B20" s="3" t="s">
         <v>73</v>
@@ -1410,7 +1430,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="15"/>
       <c r="B21" s="3" t="s">
         <v>78</v>
@@ -1428,7 +1448,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
       <c r="B22" s="3" t="s">
         <v>82</v>
@@ -1446,7 +1466,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="16"/>
       <c r="B23" s="3" t="s">
         <v>86</v>
@@ -1464,7 +1484,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="17"/>
       <c r="B24" s="3" t="s">
         <v>90</v>
@@ -1482,7 +1502,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" s="18"/>
       <c r="B25" s="3" t="s">
         <v>94</v>
@@ -1500,7 +1520,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="3" t="s">
         <v>98</v>
@@ -1518,7 +1538,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="17"/>
       <c r="B27" s="3" t="s">
         <v>102</v>
@@ -1536,7 +1556,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="20"/>
       <c r="B28" s="3" t="s">
         <v>106</v>
@@ -1554,7 +1574,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="20"/>
       <c r="B29" s="3" t="s">
         <v>110</v>
@@ -1572,7 +1592,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A30" s="21"/>
       <c r="B30" s="3" t="s">
         <v>114</v>
@@ -1590,7 +1610,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" s="21"/>
       <c r="B31" s="3" t="s">
         <v>118</v>
@@ -1608,7 +1628,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" s="21"/>
       <c r="B32" s="3" t="s">
         <v>121</v>
@@ -1626,7 +1646,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" s="21"/>
       <c r="B33" s="3" t="s">
         <v>125</v>
@@ -1644,7 +1664,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A34" s="21"/>
       <c r="B34" s="3" t="s">
         <v>129</v>
@@ -1662,7 +1682,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" s="22"/>
       <c r="B35" s="3" t="s">
         <v>133</v>
@@ -1680,7 +1700,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" s="21"/>
       <c r="B36" s="3" t="s">
         <v>137</v>
@@ -1698,7 +1718,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A37" s="22"/>
       <c r="B37" s="3" t="s">
         <v>140</v>
@@ -1716,7 +1736,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A38" s="23"/>
       <c r="B38" s="3" t="s">
         <v>144</v>
@@ -1779,844 +1799,865 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E36"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F1" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.140625" customWidth="1"/>
-    <col min="4" max="4" width="35.28515625" customWidth="1"/>
-    <col min="5" max="5" width="101.140625" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" customWidth="1"/>
+    <col min="1" max="1" width="37.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" customWidth="1"/>
+    <col min="5" max="5" width="101.109375" customWidth="1"/>
+    <col min="6" max="6" width="26.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>148</v>
       </c>
-      <c r="B1">
+      <c r="B2">
         <v>0</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1" t="str">
-        <f>UPPER(A1)</f>
-        <v>NULL_CONSEQUENCE</v>
-      </c>
-      <c r="E1" t="str">
-        <f>"{ E_"&amp;D1&amp;","""&amp;A1&amp;"""," &amp;C1 &amp;".0 },"</f>
-        <v>{ E_NULL_CONSEQUENCE,"NULL_CONSEQUENCE",1.0 },</v>
-      </c>
-      <c r="F1" t="str">
-        <f>"E_"&amp;D1&amp;","</f>
-        <v>E_NULL_CONSEQUENCE,</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D36" si="0">UPPER(A2)</f>
-        <v>INTERGENIC_VARIANT</v>
+        <f>"E_"&amp;UPPER(A2)</f>
+        <v>E_NULL_CONSEQUENCE</v>
       </c>
       <c r="E2" t="str">
-        <f t="shared" ref="E2:E36" si="1">"{ E_"&amp;D2&amp;","""&amp;A2&amp;"""," &amp;C2 &amp;".0 },"</f>
+        <f>"{ "&amp;D2&amp;","""&amp;A2&amp;"""," &amp;C2 &amp;".0 },"</f>
+        <v>{ E_NULL_CONSEQUENCE,"NULL_CONSEQUENCE",1.0 },</v>
+      </c>
+      <c r="F2" t="str">
+        <f>D2&amp;","</f>
+        <v>E_NULL_CONSEQUENCE,</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D37" si="0">"E_"&amp;UPPER(A3)</f>
+        <v>E_INTERGENIC_VARIANT</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E37" si="1">"{ "&amp;D3&amp;","""&amp;A3&amp;"""," &amp;C3 &amp;".0 },"</f>
         <v>{ E_INTERGENIC_VARIANT,"intergenic_variant",1.0 },</v>
       </c>
-      <c r="F2" t="str">
-        <f t="shared" ref="F2:F36" si="2">"E_"&amp;D2&amp;","</f>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F37" si="2">D3&amp;","</f>
         <v>E_INTERGENIC_VARIANT,</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>140</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>2</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3" t="str">
-        <f t="shared" si="0"/>
-        <v>FEATURE_TRUNCATION</v>
-      </c>
-      <c r="E3" t="str">
-        <f t="shared" si="1"/>
-        <v>{ E_FEATURE_TRUNCATION,"feature_truncation",3.0 },</v>
-      </c>
-      <c r="F3" t="str">
-        <f t="shared" si="2"/>
-        <v>E_FEATURE_TRUNCATION,</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>137</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>REGULATORY_REGION_VARIANT</v>
+        <v>E_FEATURE_TRUNCATION</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="1"/>
-        <v>{ E_REGULATORY_REGION_VARIANT,"regulatory_region_variant",3.0 },</v>
+        <v>{ E_FEATURE_TRUNCATION,"feature_truncation",3.0 },</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="2"/>
-        <v>E_REGULATORY_REGION_VARIANT,</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>E_FEATURE_TRUNCATION,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>FEATURE_ELONGATION</v>
+        <v>E_REGULATORY_REGION_VARIANT</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="1"/>
-        <v>{ E_FEATURE_ELONGATION,"feature_elongation",3.0 },</v>
+        <v>{ E_REGULATORY_REGION_VARIANT,"regulatory_region_variant",3.0 },</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="2"/>
-        <v>E_FEATURE_ELONGATION,</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>E_REGULATORY_REGION_VARIANT,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>REGULATORY_REGION_AMPLIFICATION</v>
+        <v>E_FEATURE_ELONGATION</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="1"/>
-        <v>{ E_REGULATORY_REGION_AMPLIFICATION,"regulatory_region_amplification",3.0 },</v>
+        <v>{ E_FEATURE_ELONGATION,"feature_elongation",3.0 },</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="2"/>
-        <v>E_REGULATORY_REGION_AMPLIFICATION,</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>E_FEATURE_ELONGATION,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>REGULATORY_REGION_ABLATION</v>
+        <v>E_REGULATORY_REGION_AMPLIFICATION</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="1"/>
-        <v>{ E_REGULATORY_REGION_ABLATION,"regulatory_region_ablation",3.0 },</v>
+        <v>{ E_REGULATORY_REGION_AMPLIFICATION,"regulatory_region_amplification",3.0 },</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="2"/>
-        <v>E_REGULATORY_REGION_ABLATION,</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>E_REGULATORY_REGION_AMPLIFICATION,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>TF_BINDING_SITE_VARIANT</v>
+        <v>E_REGULATORY_REGION_ABLATION</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="1"/>
-        <v>{ E_TF_BINDING_SITE_VARIANT,"TF_binding_site_variant",3.0 },</v>
+        <v>{ E_REGULATORY_REGION_ABLATION,"regulatory_region_ablation",3.0 },</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="2"/>
-        <v>E_TF_BINDING_SITE_VARIANT,</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>E_REGULATORY_REGION_ABLATION,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>TFBS_AMPLIFICATION</v>
+        <v>E_TF_BINDING_SITE_VARIANT</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="1"/>
-        <v>{ E_TFBS_AMPLIFICATION,"TFBS_amplification",3.0 },</v>
+        <v>{ E_TF_BINDING_SITE_VARIANT,"TF_binding_site_variant",3.0 },</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="2"/>
-        <v>E_TFBS_AMPLIFICATION,</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>E_TF_BINDING_SITE_VARIANT,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10">
         <v>3</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>TFBS_ABLATION</v>
+        <v>E_TFBS_AMPLIFICATION</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="1"/>
-        <v>{ E_TFBS_ABLATION,"TFBS_ablation",3.0 },</v>
+        <v>{ E_TFBS_AMPLIFICATION,"TFBS_amplification",3.0 },</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="2"/>
-        <v>E_TFBS_ABLATION,</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>E_TFBS_AMPLIFICATION,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11">
         <v>3</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>DOWNSTREAM_GENE_VARIANT</v>
+        <v>E_TFBS_ABLATION</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="1"/>
-        <v>{ E_DOWNSTREAM_GENE_VARIANT,"downstream_gene_variant",3.0 },</v>
+        <v>{ E_TFBS_ABLATION,"TFBS_ablation",3.0 },</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="2"/>
-        <v>E_DOWNSTREAM_GENE_VARIANT,</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>E_TFBS_ABLATION,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>UPSTREAM_GENE_VARIANT</v>
+        <v>E_DOWNSTREAM_GENE_VARIANT</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="1"/>
-        <v>{ E_UPSTREAM_GENE_VARIANT,"upstream_gene_variant",3.0 },</v>
+        <v>{ E_DOWNSTREAM_GENE_VARIANT,"downstream_gene_variant",3.0 },</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="2"/>
-        <v>E_UPSTREAM_GENE_VARIANT,</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>E_DOWNSTREAM_GENE_VARIANT,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13">
         <v>3</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>NON_CODING_TRANSCRIPT_VARIANT</v>
+        <v>E_UPSTREAM_GENE_VARIANT</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="1"/>
-        <v>{ E_NON_CODING_TRANSCRIPT_VARIANT,"non_coding_transcript_variant",3.0 },</v>
+        <v>{ E_UPSTREAM_GENE_VARIANT,"upstream_gene_variant",3.0 },</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="2"/>
-        <v>E_NON_CODING_TRANSCRIPT_VARIANT,</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>E_UPSTREAM_GENE_VARIANT,</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14">
         <v>3</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>NMD_TRANSCRIPT_VARIANT</v>
+        <v>E_NON_CODING_TRANSCRIPT_VARIANT</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="1"/>
-        <v>{ E_NMD_TRANSCRIPT_VARIANT,"NMD_transcript_variant",3.0 },</v>
+        <v>{ E_NON_CODING_TRANSCRIPT_VARIANT,"non_coding_transcript_variant",3.0 },</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="2"/>
-        <v>E_NMD_TRANSCRIPT_VARIANT,</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>E_NON_CODING_TRANSCRIPT_VARIANT,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15">
         <v>3</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>INTRON_VARIANT</v>
+        <v>E_NMD_TRANSCRIPT_VARIANT</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="1"/>
-        <v>{ E_INTRON_VARIANT,"intron_variant",3.0 },</v>
+        <v>{ E_NMD_TRANSCRIPT_VARIANT,"NMD_transcript_variant",3.0 },</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="2"/>
-        <v>E_INTRON_VARIANT,</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>E_NMD_TRANSCRIPT_VARIANT,</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16">
         <v>3</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>NON_CODING_TRANSCRIPT_EXON_VARIANT</v>
+        <v>E_INTRON_VARIANT</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="1"/>
+        <v>{ E_INTRON_VARIANT,"intron_variant",3.0 },</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="2"/>
+        <v>E_INTRON_VARIANT,</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>E_NON_CODING_TRANSCRIPT_EXON_VARIANT</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="1"/>
         <v>{ E_NON_CODING_TRANSCRIPT_EXON_VARIANT,"non_coding_transcript_exon_variant",3.0 },</v>
       </c>
-      <c r="F16" t="str">
+      <c r="F17" t="str">
         <f t="shared" si="2"/>
         <v>E_NON_CODING_TRANSCRIPT_EXON_VARIANT,</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>86</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>16</v>
-      </c>
-      <c r="C17">
-        <v>5</v>
-      </c>
-      <c r="D17" t="str">
-        <f t="shared" si="0"/>
-        <v>3_PRIME_UTR_VARIANT</v>
-      </c>
-      <c r="E17" t="str">
-        <f t="shared" si="1"/>
-        <v>{ E_3_PRIME_UTR_VARIANT,"3_prime_UTR_variant",5.0 },</v>
-      </c>
-      <c r="F17" t="str">
-        <f t="shared" si="2"/>
-        <v>E_3_PRIME_UTR_VARIANT,</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>82</v>
-      </c>
-      <c r="B18">
-        <v>17</v>
       </c>
       <c r="C18">
         <v>5</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>5_PRIME_UTR_VARIANT</v>
+        <v>E_3_PRIME_UTR_VARIANT</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="1"/>
-        <v>{ E_5_PRIME_UTR_VARIANT,"5_prime_UTR_variant",5.0 },</v>
+        <v>{ E_3_PRIME_UTR_VARIANT,"3_prime_UTR_variant",5.0 },</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="2"/>
-        <v>E_5_PRIME_UTR_VARIANT,</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>E_3_PRIME_UTR_VARIANT,</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19">
         <v>5</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>MATURE_MIRNA_VARIANT</v>
+        <v>E_5_PRIME_UTR_VARIANT</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="1"/>
-        <v>{ E_MATURE_MIRNA_VARIANT,"mature_miRNA_variant",5.0 },</v>
+        <v>{ E_5_PRIME_UTR_VARIANT,"5_prime_UTR_variant",5.0 },</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="2"/>
-        <v>E_MATURE_MIRNA_VARIANT,</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>E_5_PRIME_UTR_VARIANT,</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20">
         <v>5</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>CODING_SEQUENCE_VARIANT</v>
+        <v>E_MATURE_MIRNA_VARIANT</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="1"/>
-        <v>{ E_CODING_SEQUENCE_VARIANT,"coding_sequence_variant",5.0 },</v>
+        <v>{ E_MATURE_MIRNA_VARIANT,"mature_miRNA_variant",5.0 },</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="2"/>
-        <v>E_CODING_SEQUENCE_VARIANT,</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>E_MATURE_MIRNA_VARIANT,</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21">
         <v>5</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>SYNONYMOUS_VARIANT</v>
+        <v>E_CODING_SEQUENCE_VARIANT</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="1"/>
-        <v>{ E_SYNONYMOUS_VARIANT,"synonymous_variant",5.0 },</v>
+        <v>{ E_CODING_SEQUENCE_VARIANT,"coding_sequence_variant",5.0 },</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="2"/>
-        <v>E_SYNONYMOUS_VARIANT,</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>E_CODING_SEQUENCE_VARIANT,</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22">
         <v>5</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>STOP_RETAINED_VARIANT</v>
+        <v>E_SYNONYMOUS_VARIANT</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="1"/>
-        <v>{ E_STOP_RETAINED_VARIANT,"stop_retained_variant",5.0 },</v>
+        <v>{ E_SYNONYMOUS_VARIANT,"synonymous_variant",5.0 },</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="2"/>
-        <v>E_STOP_RETAINED_VARIANT,</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>E_SYNONYMOUS_VARIANT,</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23">
         <v>5</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>INCOMPLETE_TERMINAL_CODON_VARIANT</v>
+        <v>E_STOP_RETAINED_VARIANT</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="1"/>
-        <v>{ E_INCOMPLETE_TERMINAL_CODON_VARIANT,"incomplete_terminal_codon_variant",5.0 },</v>
+        <v>{ E_STOP_RETAINED_VARIANT,"stop_retained_variant",5.0 },</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="2"/>
-        <v>E_INCOMPLETE_TERMINAL_CODON_VARIANT,</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>E_STOP_RETAINED_VARIANT,</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C24">
         <v>5</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v>SPLICE_REGION_VARIANT</v>
+        <v>E_INCOMPLETE_TERMINAL_CODON_VARIANT</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="1"/>
+        <v>{ E_INCOMPLETE_TERMINAL_CODON_VARIANT,"incomplete_terminal_codon_variant",5.0 },</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="2"/>
+        <v>E_INCOMPLETE_TERMINAL_CODON_VARIANT,</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25">
+        <v>23</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>E_SPLICE_REGION_VARIANT</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="1"/>
         <v>{ E_SPLICE_REGION_VARIANT,"splice_region_variant",5.0 },</v>
       </c>
-      <c r="F24" t="str">
+      <c r="F25" t="str">
         <f t="shared" si="2"/>
         <v>E_SPLICE_REGION_VARIANT,</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>52</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <v>24</v>
-      </c>
-      <c r="C25">
-        <v>10</v>
-      </c>
-      <c r="D25" t="str">
-        <f t="shared" si="0"/>
-        <v>PROTEIN_ALTERING_VARIANT</v>
-      </c>
-      <c r="E25" t="str">
-        <f t="shared" si="1"/>
-        <v>{ E_PROTEIN_ALTERING_VARIANT,"protein_altering_variant",10.0 },</v>
-      </c>
-      <c r="F25" t="str">
-        <f t="shared" si="2"/>
-        <v>E_PROTEIN_ALTERING_VARIANT,</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26">
-        <v>25</v>
       </c>
       <c r="C26">
         <v>10</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
-        <v>MISSENSE_VARIANT</v>
+        <v>E_PROTEIN_ALTERING_VARIANT</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="1"/>
+        <v>{ E_PROTEIN_ALTERING_VARIANT,"protein_altering_variant",10.0 },</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="2"/>
+        <v>E_PROTEIN_ALTERING_VARIANT,</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27">
+        <v>25</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>E_MISSENSE_VARIANT</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="1"/>
         <v>{ E_MISSENSE_VARIANT,"missense_variant",10.0 },</v>
       </c>
-      <c r="F26" t="str">
+      <c r="F27" t="str">
         <f t="shared" si="2"/>
         <v>E_MISSENSE_VARIANT,</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>44</v>
       </c>
-      <c r="B27">
+      <c r="B28">
         <v>26</v>
-      </c>
-      <c r="C27">
-        <v>15</v>
-      </c>
-      <c r="D27" t="str">
-        <f t="shared" si="0"/>
-        <v>INFRAME_DELETION</v>
-      </c>
-      <c r="E27" t="str">
-        <f t="shared" si="1"/>
-        <v>{ E_INFRAME_DELETION,"inframe_deletion",15.0 },</v>
-      </c>
-      <c r="F27" t="str">
-        <f t="shared" si="2"/>
-        <v>E_INFRAME_DELETION,</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28">
-        <v>27</v>
       </c>
       <c r="C28">
         <v>15</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
-        <v>INFRAME_INSERTION</v>
+        <v>E_INFRAME_DELETION</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="1"/>
-        <v>{ E_INFRAME_INSERTION,"inframe_insertion",15.0 },</v>
+        <v>{ E_INFRAME_DELETION,"inframe_deletion",15.0 },</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="2"/>
-        <v>E_INFRAME_INSERTION,</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>E_INFRAME_DELETION,</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C29">
         <v>15</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
-        <v>TRANSCRIPT_AMPLIFICATION</v>
+        <v>E_INFRAME_INSERTION</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="1"/>
-        <v>{ E_TRANSCRIPT_AMPLIFICATION,"transcript_amplification",15.0 },</v>
+        <v>{ E_INFRAME_INSERTION,"inframe_insertion",15.0 },</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="2"/>
-        <v>E_TRANSCRIPT_AMPLIFICATION,</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>E_INFRAME_INSERTION,</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C30">
         <v>15</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
-        <v>START_LOST</v>
+        <v>E_TRANSCRIPT_AMPLIFICATION</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="1"/>
-        <v>{ E_START_LOST,"start_lost",15.0 },</v>
+        <v>{ E_TRANSCRIPT_AMPLIFICATION,"transcript_amplification",15.0 },</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="2"/>
-        <v>E_START_LOST,</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>E_TRANSCRIPT_AMPLIFICATION,</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C31">
         <v>15</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
-        <v>STOP_LOST</v>
+        <v>E_START_LOST</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="1"/>
+        <v>{ E_START_LOST,"start_lost",15.0 },</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="2"/>
+        <v>E_START_LOST,</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32">
+        <v>30</v>
+      </c>
+      <c r="C32">
+        <v>15</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>E_STOP_LOST</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="1"/>
         <v>{ E_STOP_LOST,"stop_lost",15.0 },</v>
       </c>
-      <c r="F31" t="str">
+      <c r="F32" t="str">
         <f t="shared" si="2"/>
         <v>E_STOP_LOST,</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>23</v>
       </c>
-      <c r="B32">
+      <c r="B33">
         <v>31</v>
-      </c>
-      <c r="C32">
-        <v>20</v>
-      </c>
-      <c r="D32" t="str">
-        <f t="shared" si="0"/>
-        <v>FRAMESHIFT_VARIANT</v>
-      </c>
-      <c r="E32" t="str">
-        <f t="shared" si="1"/>
-        <v>{ E_FRAMESHIFT_VARIANT,"frameshift_variant",20.0 },</v>
-      </c>
-      <c r="F32" t="str">
-        <f t="shared" si="2"/>
-        <v>E_FRAMESHIFT_VARIANT,</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>19</v>
-      </c>
-      <c r="B33">
-        <v>32</v>
       </c>
       <c r="C33">
         <v>20</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
-        <v>STOP_GAINED</v>
+        <v>E_FRAMESHIFT_VARIANT</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="1"/>
-        <v>{ E_STOP_GAINED,"stop_gained",20.0 },</v>
+        <v>{ E_FRAMESHIFT_VARIANT,"frameshift_variant",20.0 },</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="2"/>
-        <v>E_STOP_GAINED,</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>E_FRAMESHIFT_VARIANT,</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B34">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C34">
         <v>20</v>
       </c>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
-        <v>SPLICE_DONOR_VARIANT</v>
+        <v>E_STOP_GAINED</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" si="1"/>
-        <v>{ E_SPLICE_DONOR_VARIANT,"splice_donor_variant",20.0 },</v>
+        <v>{ E_STOP_GAINED,"stop_gained",20.0 },</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="2"/>
-        <v>E_SPLICE_DONOR_VARIANT,</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>E_STOP_GAINED,</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B35">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C35">
         <v>20</v>
       </c>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
-        <v>SPLICE_ACCEPTOR_VARIANT</v>
+        <v>E_SPLICE_DONOR_VARIANT</v>
       </c>
       <c r="E35" t="str">
         <f t="shared" si="1"/>
-        <v>{ E_SPLICE_ACCEPTOR_VARIANT,"splice_acceptor_variant",20.0 },</v>
+        <v>{ E_SPLICE_DONOR_VARIANT,"splice_donor_variant",20.0 },</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="2"/>
-        <v>E_SPLICE_ACCEPTOR_VARIANT,</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>E_SPLICE_DONOR_VARIANT,</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B36">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C36">
         <v>20</v>
       </c>
       <c r="D36" t="str">
         <f t="shared" si="0"/>
-        <v>TRANSCRIPT_ABLATION</v>
+        <v>E_SPLICE_ACCEPTOR_VARIANT</v>
       </c>
       <c r="E36" t="str">
         <f t="shared" si="1"/>
+        <v>{ E_SPLICE_ACCEPTOR_VARIANT,"splice_acceptor_variant",20.0 },</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="2"/>
+        <v>E_SPLICE_ACCEPTOR_VARIANT,</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37">
+        <v>35</v>
+      </c>
+      <c r="C37">
+        <v>20</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>E_TRANSCRIPT_ABLATION</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="1"/>
         <v>{ E_TRANSCRIPT_ABLATION,"transcript_ablation",20.0 },</v>
       </c>
-      <c r="F36" t="str">
+      <c r="F37" t="str">
         <f t="shared" si="2"/>
         <v>E_TRANSCRIPT_ABLATION,</v>
       </c>
@@ -2631,386 +2672,962 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.5546875" customWidth="1"/>
+    <col min="4" max="4" width="44.109375" customWidth="1"/>
+    <col min="5" max="5" width="67.6640625" customWidth="1"/>
+    <col min="6" max="6" width="33.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="str">
+        <f>UPPER(A2)</f>
+        <v>NULL_CONSEQUENCE</v>
+      </c>
+      <c r="E2" t="str">
+        <f>"{ "&amp;D2&amp;","""&amp;A2&amp;"""," &amp;C2 &amp;".0 },"</f>
+        <v>{ NULL_CONSEQUENCE,"NULL_CONSEQUENCE",1.0 },</v>
+      </c>
+      <c r="F2" t="str">
+        <f>D2&amp;","</f>
+        <v>NULL_CONSEQUENCE,</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D17" si="0">UPPER(A3)</f>
+        <v>INTERGENIC</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E17" si="1">"{ "&amp;D3&amp;","""&amp;A3&amp;"""," &amp;C3 &amp;".0 },"</f>
+        <v>{ INTERGENIC,"INTERGENIC",1.0 },</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F17" si="2">D3&amp;","</f>
+        <v>INTERGENIC,</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>DOWNSTREAM</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="1"/>
+        <v>{ DOWNSTREAM,"DOWNSTREAM",1.0 },</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="2"/>
+        <v>DOWNSTREAM,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>INTRONIC</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="1"/>
+        <v>{ INTRONIC,"INTRONIC",3.0 },</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="2"/>
+        <v>INTRONIC,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>THREEPRIME_UTR</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>{ THREEPRIME_UTR,"THREEPRIME_UTR",5.0 },</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="2"/>
+        <v>THREEPRIME_UTR,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>UPSTREAM</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>{ UPSTREAM,"UPSTREAM",5.0 },</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="2"/>
+        <v>UPSTREAM,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>SYNONYMOUS_CODING</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>{ SYNONYMOUS_CODING,"SYNONYMOUS_CODING",3.0 },</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="2"/>
+        <v>SYNONYMOUS_CODING,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>FIVEPRIME_UTR</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>{ FIVEPRIME_UTR,"FIVEPRIME_UTR",5.0 },</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="2"/>
+        <v>FIVEPRIME_UTR,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>15</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>CODINGINDEL</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>{ CODINGINDEL,"CODINGINDEL",15.0 },</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="2"/>
+        <v>CODINGINDEL,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>157</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>SPLICE_SITE</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>{ SPLICE_SITE,"SPLICE_SITE",5.0 },</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="2"/>
+        <v>SPLICE_SITE,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>158</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>STOP_LOST</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>{ STOP_LOST,"STOP_LOST",5.0 },</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="2"/>
+        <v>STOP_LOST,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>159</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>NON_SYNONYMOUS_CODING</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>{ NON_SYNONYMOUS_CODING,"NON_SYNONYMOUS_CODING",10.0 },</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="2"/>
+        <v>NON_SYNONYMOUS_CODING,</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>160</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>20</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>FRAMESHIFT_CODING</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>{ FRAMESHIFT_CODING,"FRAMESHIFT_CODING",20.0 },</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="2"/>
+        <v>FRAMESHIFT_CODING,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>ESSENTIAL_SPLICE_SITE</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>{ ESSENTIAL_SPLICE_SITE,"ESSENTIAL_SPLICE_SITE",10.0 },</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="2"/>
+        <v>ESSENTIAL_SPLICE_SITE,</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>162</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>20</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>STOP_GAINED</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>{ STOP_GAINED,"STOP_GAINED",20.0 },</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="2"/>
+        <v>STOP_GAINED,</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>163</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>KOZAK</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v>{ KOZAK,"KOZAK",10.0 },</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="2"/>
+        <v>KOZAK,</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B2" sqref="A2:B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="44.140625" customWidth="1"/>
-    <col min="5" max="5" width="67.7109375" customWidth="1"/>
-    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="1" max="1" width="35.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>148</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="str">
+        <f>Sheet2!A2</f>
+        <v>NULL_CONSEQUENCE</v>
       </c>
       <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
+        <f>Sheet2!C2</f>
         <v>1</v>
       </c>
-      <c r="D1" t="str">
-        <f>UPPER(A1)</f>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="str">
+        <f>Sheet2!A3</f>
+        <v>intergenic_variant</v>
+      </c>
+      <c r="B2">
+        <f>Sheet2!C3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <f>Sheet2!A4</f>
+        <v>feature_truncation</v>
+      </c>
+      <c r="B3">
+        <f>Sheet2!C4</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <f>Sheet2!A5</f>
+        <v>regulatory_region_variant</v>
+      </c>
+      <c r="B4">
+        <f>Sheet2!C5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <f>Sheet2!A6</f>
+        <v>feature_elongation</v>
+      </c>
+      <c r="B5">
+        <f>Sheet2!C6</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
+        <f>Sheet2!A7</f>
+        <v>regulatory_region_amplification</v>
+      </c>
+      <c r="B6">
+        <f>Sheet2!C7</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
+        <f>Sheet2!A8</f>
+        <v>regulatory_region_ablation</v>
+      </c>
+      <c r="B7">
+        <f>Sheet2!C8</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="str">
+        <f>Sheet2!A9</f>
+        <v>TF_binding_site_variant</v>
+      </c>
+      <c r="B8">
+        <f>Sheet2!C9</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="str">
+        <f>Sheet2!A10</f>
+        <v>TFBS_amplification</v>
+      </c>
+      <c r="B9">
+        <f>Sheet2!C10</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="str">
+        <f>Sheet2!A11</f>
+        <v>TFBS_ablation</v>
+      </c>
+      <c r="B10">
+        <f>Sheet2!C11</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="str">
+        <f>Sheet2!A12</f>
+        <v>downstream_gene_variant</v>
+      </c>
+      <c r="B11">
+        <f>Sheet2!C12</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="str">
+        <f>Sheet2!A13</f>
+        <v>upstream_gene_variant</v>
+      </c>
+      <c r="B12">
+        <f>Sheet2!C13</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="str">
+        <f>Sheet2!A14</f>
+        <v>non_coding_transcript_variant</v>
+      </c>
+      <c r="B13">
+        <f>Sheet2!C14</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="str">
+        <f>Sheet2!A15</f>
+        <v>NMD_transcript_variant</v>
+      </c>
+      <c r="B14">
+        <f>Sheet2!C15</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="str">
+        <f>Sheet2!A16</f>
+        <v>intron_variant</v>
+      </c>
+      <c r="B15">
+        <f>Sheet2!C16</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="str">
+        <f>Sheet2!A17</f>
+        <v>non_coding_transcript_exon_variant</v>
+      </c>
+      <c r="B16">
+        <f>Sheet2!C17</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="str">
+        <f>Sheet2!A18</f>
+        <v>3_prime_UTR_variant</v>
+      </c>
+      <c r="B17">
+        <f>Sheet2!C18</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="str">
+        <f>Sheet2!A19</f>
+        <v>5_prime_UTR_variant</v>
+      </c>
+      <c r="B18">
+        <f>Sheet2!C19</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="str">
+        <f>Sheet2!A20</f>
+        <v>mature_miRNA_variant</v>
+      </c>
+      <c r="B19">
+        <f>Sheet2!C20</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="str">
+        <f>Sheet2!A21</f>
+        <v>coding_sequence_variant</v>
+      </c>
+      <c r="B20">
+        <f>Sheet2!C21</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="str">
+        <f>Sheet2!A22</f>
+        <v>synonymous_variant</v>
+      </c>
+      <c r="B21">
+        <f>Sheet2!C22</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="str">
+        <f>Sheet2!A23</f>
+        <v>stop_retained_variant</v>
+      </c>
+      <c r="B22">
+        <f>Sheet2!C23</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="str">
+        <f>Sheet2!A24</f>
+        <v>incomplete_terminal_codon_variant</v>
+      </c>
+      <c r="B23">
+        <f>Sheet2!C24</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="str">
+        <f>Sheet2!A25</f>
+        <v>splice_region_variant</v>
+      </c>
+      <c r="B24">
+        <f>Sheet2!C25</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="str">
+        <f>Sheet2!A26</f>
+        <v>protein_altering_variant</v>
+      </c>
+      <c r="B25">
+        <f>Sheet2!C26</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="str">
+        <f>Sheet2!A27</f>
+        <v>missense_variant</v>
+      </c>
+      <c r="B26">
+        <f>Sheet2!C27</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="str">
+        <f>Sheet2!A28</f>
+        <v>inframe_deletion</v>
+      </c>
+      <c r="B27">
+        <f>Sheet2!C28</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="str">
+        <f>Sheet2!A29</f>
+        <v>inframe_insertion</v>
+      </c>
+      <c r="B28">
+        <f>Sheet2!C29</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="str">
+        <f>Sheet2!A30</f>
+        <v>transcript_amplification</v>
+      </c>
+      <c r="B29">
+        <f>Sheet2!C30</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="str">
+        <f>Sheet2!A31</f>
+        <v>start_lost</v>
+      </c>
+      <c r="B30">
+        <f>Sheet2!C31</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="str">
+        <f>Sheet2!A32</f>
+        <v>stop_lost</v>
+      </c>
+      <c r="B31">
+        <f>Sheet2!C32</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="str">
+        <f>Sheet2!A33</f>
+        <v>frameshift_variant</v>
+      </c>
+      <c r="B32">
+        <f>Sheet2!C33</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="str">
+        <f>Sheet2!A34</f>
+        <v>stop_gained</v>
+      </c>
+      <c r="B33">
+        <f>Sheet2!C34</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="str">
+        <f>Sheet2!A35</f>
+        <v>splice_donor_variant</v>
+      </c>
+      <c r="B34">
+        <f>Sheet2!C35</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="str">
+        <f>Sheet2!A36</f>
+        <v>splice_acceptor_variant</v>
+      </c>
+      <c r="B35">
+        <f>Sheet2!C36</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="str">
+        <f>Sheet2!A37</f>
+        <v>transcript_ablation</v>
+      </c>
+      <c r="B36">
+        <f>Sheet2!C37</f>
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="str">
+        <f>Sheet3!A2</f>
         <v>NULL_CONSEQUENCE</v>
       </c>
-      <c r="E1" t="str">
-        <f>"{ "&amp;D1&amp;","""&amp;A1&amp;"""," &amp;C1 &amp;".0 },"</f>
-        <v>{ NULL_CONSEQUENCE,"NULL_CONSEQUENCE",1.0 },</v>
-      </c>
-      <c r="F1" t="str">
-        <f>D1&amp;","</f>
-        <v>NULL_CONSEQUENCE,</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>149</v>
+      <c r="B1">
+        <f>Sheet3!C2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="str">
+        <f>Sheet3!A3</f>
+        <v>INTERGENIC</v>
       </c>
       <c r="B2">
+        <f>Sheet3!C3</f>
         <v>1</v>
       </c>
-      <c r="C2">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <f>Sheet3!A4</f>
+        <v>DOWNSTREAM</v>
+      </c>
+      <c r="B3">
+        <f>Sheet3!C4</f>
         <v>1</v>
       </c>
-      <c r="D2" t="str">
-        <f t="shared" ref="D2:D16" si="0">UPPER(A2)</f>
-        <v>INTERGENIC</v>
-      </c>
-      <c r="E2" t="str">
-        <f t="shared" ref="E2:E16" si="1">"{ "&amp;D2&amp;","""&amp;A2&amp;"""," &amp;C2 &amp;".0 },"</f>
-        <v>{ INTERGENIC,"INTERGENIC",1.0 },</v>
-      </c>
-      <c r="F2" t="str">
-        <f t="shared" ref="F2:F16" si="2">D2&amp;","</f>
-        <v>INTERGENIC,</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="str">
-        <f t="shared" si="0"/>
-        <v>DOWNSTREAM</v>
-      </c>
-      <c r="E3" t="str">
-        <f t="shared" si="1"/>
-        <v>{ DOWNSTREAM,"DOWNSTREAM",1.0 },</v>
-      </c>
-      <c r="F3" t="str">
-        <f t="shared" si="2"/>
-        <v>DOWNSTREAM,</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>151</v>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <f>Sheet3!A5</f>
+        <v>INTRONIC</v>
       </c>
       <c r="B4">
+        <f>Sheet3!C5</f>
         <v>3</v>
       </c>
-      <c r="C4">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <f>Sheet3!A6</f>
+        <v>THREEPRIME_UTR</v>
+      </c>
+      <c r="B5">
+        <f>Sheet3!C6</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
+        <f>Sheet3!A7</f>
+        <v>UPSTREAM</v>
+      </c>
+      <c r="B6">
+        <f>Sheet3!C7</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
+        <f>Sheet3!A8</f>
+        <v>SYNONYMOUS_CODING</v>
+      </c>
+      <c r="B7">
+        <f>Sheet3!C8</f>
         <v>3</v>
       </c>
-      <c r="D4" t="str">
-        <f t="shared" si="0"/>
-        <v>INTRONIC</v>
-      </c>
-      <c r="E4" t="str">
-        <f t="shared" si="1"/>
-        <v>{ INTRONIC,"INTRONIC",3.0 },</v>
-      </c>
-      <c r="F4" t="str">
-        <f t="shared" si="2"/>
-        <v>INTRONIC,</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>152</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="str">
+        <f>Sheet3!A9</f>
+        <v>FIVEPRIME_UTR</v>
+      </c>
+      <c r="B8">
+        <f>Sheet3!C9</f>
         <v>5</v>
       </c>
-      <c r="D5" t="str">
-        <f t="shared" si="0"/>
-        <v>THREEPRIME_UTR</v>
-      </c>
-      <c r="E5" t="str">
-        <f t="shared" si="1"/>
-        <v>{ THREEPRIME_UTR,"THREEPRIME_UTR",5.0 },</v>
-      </c>
-      <c r="F5" t="str">
-        <f t="shared" si="2"/>
-        <v>THREEPRIME_UTR,</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>153</v>
-      </c>
-      <c r="B6">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="str">
+        <f>Sheet3!A10</f>
+        <v>CODINGINDEL</v>
+      </c>
+      <c r="B9">
+        <f>Sheet3!C10</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="str">
+        <f>Sheet3!A11</f>
+        <v>SPLICE_SITE</v>
+      </c>
+      <c r="B10">
+        <f>Sheet3!C11</f>
         <v>5</v>
       </c>
-      <c r="C6">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="str">
+        <f>Sheet3!A12</f>
+        <v>STOP_LOST</v>
+      </c>
+      <c r="B11">
+        <f>Sheet3!C12</f>
         <v>5</v>
       </c>
-      <c r="D6" t="str">
-        <f t="shared" si="0"/>
-        <v>UPSTREAM</v>
-      </c>
-      <c r="E6" t="str">
-        <f t="shared" si="1"/>
-        <v>{ UPSTREAM,"UPSTREAM",5.0 },</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" si="2"/>
-        <v>UPSTREAM,</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>154</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" si="0"/>
-        <v>SYNONYMOUS_CODING</v>
-      </c>
-      <c r="E7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ SYNONYMOUS_CODING,"SYNONYMOUS_CODING",3.0 },</v>
-      </c>
-      <c r="F7" t="str">
-        <f t="shared" si="2"/>
-        <v>SYNONYMOUS_CODING,</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>155</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8" t="str">
-        <f t="shared" si="0"/>
-        <v>FIVEPRIME_UTR</v>
-      </c>
-      <c r="E8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ FIVEPRIME_UTR,"FIVEPRIME_UTR",5.0 },</v>
-      </c>
-      <c r="F8" t="str">
-        <f t="shared" si="2"/>
-        <v>FIVEPRIME_UTR,</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>156</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <v>15</v>
-      </c>
-      <c r="D9" t="str">
-        <f t="shared" si="0"/>
-        <v>CODINGINDEL</v>
-      </c>
-      <c r="E9" t="str">
-        <f t="shared" si="1"/>
-        <v>{ CODINGINDEL,"CODINGINDEL",15.0 },</v>
-      </c>
-      <c r="F9" t="str">
-        <f t="shared" si="2"/>
-        <v>CODINGINDEL,</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>157</v>
-      </c>
-      <c r="B10">
-        <v>9</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10" t="str">
-        <f t="shared" si="0"/>
-        <v>SPLICE_SITE</v>
-      </c>
-      <c r="E10" t="str">
-        <f t="shared" si="1"/>
-        <v>{ SPLICE_SITE,"SPLICE_SITE",5.0 },</v>
-      </c>
-      <c r="F10" t="str">
-        <f t="shared" si="2"/>
-        <v>SPLICE_SITE,</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>158</v>
-      </c>
-      <c r="B11">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="str">
+        <f>Sheet3!A13</f>
+        <v>NON_SYNONYMOUS_CODING</v>
+      </c>
+      <c r="B12">
+        <f>Sheet3!C13</f>
         <v>10</v>
       </c>
-      <c r="C11">
-        <v>5</v>
-      </c>
-      <c r="D11" t="str">
-        <f t="shared" si="0"/>
-        <v>STOP_LOST</v>
-      </c>
-      <c r="E11" t="str">
-        <f t="shared" si="1"/>
-        <v>{ STOP_LOST,"STOP_LOST",5.0 },</v>
-      </c>
-      <c r="F11" t="str">
-        <f t="shared" si="2"/>
-        <v>STOP_LOST,</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>159</v>
-      </c>
-      <c r="B12">
-        <v>11</v>
-      </c>
-      <c r="C12">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="str">
+        <f>Sheet3!A14</f>
+        <v>FRAMESHIFT_CODING</v>
+      </c>
+      <c r="B13">
+        <f>Sheet3!C14</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="str">
+        <f>Sheet3!A15</f>
+        <v>ESSENTIAL_SPLICE_SITE</v>
+      </c>
+      <c r="B14">
+        <f>Sheet3!C15</f>
         <v>10</v>
       </c>
-      <c r="D12" t="str">
-        <f t="shared" si="0"/>
-        <v>NON_SYNONYMOUS_CODING</v>
-      </c>
-      <c r="E12" t="str">
-        <f t="shared" si="1"/>
-        <v>{ NON_SYNONYMOUS_CODING,"NON_SYNONYMOUS_CODING",10.0 },</v>
-      </c>
-      <c r="F12" t="str">
-        <f t="shared" si="2"/>
-        <v>NON_SYNONYMOUS_CODING,</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>160</v>
-      </c>
-      <c r="B13">
-        <v>12</v>
-      </c>
-      <c r="C13">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="str">
+        <f>Sheet3!A16</f>
+        <v>STOP_GAINED</v>
+      </c>
+      <c r="B15">
+        <f>Sheet3!C16</f>
         <v>20</v>
       </c>
-      <c r="D13" t="str">
-        <f t="shared" si="0"/>
-        <v>FRAMESHIFT_CODING</v>
-      </c>
-      <c r="E13" t="str">
-        <f t="shared" si="1"/>
-        <v>{ FRAMESHIFT_CODING,"FRAMESHIFT_CODING",20.0 },</v>
-      </c>
-      <c r="F13" t="str">
-        <f t="shared" si="2"/>
-        <v>FRAMESHIFT_CODING,</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>161</v>
-      </c>
-      <c r="B14">
-        <v>13</v>
-      </c>
-      <c r="C14">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="str">
+        <f>Sheet3!A17</f>
+        <v>KOZAK</v>
+      </c>
+      <c r="B16">
+        <f>Sheet3!C17</f>
         <v>10</v>
-      </c>
-      <c r="D14" t="str">
-        <f t="shared" si="0"/>
-        <v>ESSENTIAL_SPLICE_SITE</v>
-      </c>
-      <c r="E14" t="str">
-        <f t="shared" si="1"/>
-        <v>{ ESSENTIAL_SPLICE_SITE,"ESSENTIAL_SPLICE_SITE",10.0 },</v>
-      </c>
-      <c r="F14" t="str">
-        <f t="shared" si="2"/>
-        <v>ESSENTIAL_SPLICE_SITE,</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>162</v>
-      </c>
-      <c r="B15">
-        <v>14</v>
-      </c>
-      <c r="C15">
-        <v>20</v>
-      </c>
-      <c r="D15" t="str">
-        <f t="shared" si="0"/>
-        <v>STOP_GAINED</v>
-      </c>
-      <c r="E15" t="str">
-        <f t="shared" si="1"/>
-        <v>{ STOP_GAINED,"STOP_GAINED",20.0 },</v>
-      </c>
-      <c r="F15" t="str">
-        <f t="shared" si="2"/>
-        <v>STOP_GAINED,</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>163</v>
-      </c>
-      <c r="B16">
-        <v>15</v>
-      </c>
-      <c r="C16">
-        <v>10</v>
-      </c>
-      <c r="D16" t="str">
-        <f t="shared" si="0"/>
-        <v>KOZAK</v>
-      </c>
-      <c r="E16" t="str">
-        <f t="shared" si="1"/>
-        <v>{ KOZAK,"KOZAK",10.0 },</v>
-      </c>
-      <c r="F16" t="str">
-        <f t="shared" si="2"/>
-        <v>KOZAK,</v>
       </c>
     </row>
   </sheetData>

</xml_diff>